<commit_message>
Some corrections in Test-cases
</commit_message>
<xml_diff>
--- a/Test_cases.xlsx
+++ b/Test_cases.xlsx
@@ -243,6 +243,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">龍門大酒家
 </t>
@@ -562,6 +563,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -744,17 +746,17 @@
   <dimension ref="A1:G984"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="47.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="47.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="37.76"/>
   </cols>
   <sheetData>
@@ -762,7 +764,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>